<commit_message>
Verbindung zwischen Android und Firebase getestet
</commit_message>
<xml_diff>
--- a/Artefakte/ProjektplanV0.24.xlsx
+++ b/Artefakte/ProjektplanV0.24.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studium\6. Semester\EIS\EISSS19SchoenbergerTissen\Artefakte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACB2F548-DF30-4617-A523-7655045192F6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A995012D-0869-42EB-A636-131B4F2E8790}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7950" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{49FFB486-0252-4090-A15B-F7AC9F70B8C0}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="70">
   <si>
     <t>EIS Projektplan von Malte Schönberger und Arthur Tissen</t>
   </si>
@@ -452,7 +452,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -503,6 +503,7 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="8" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -819,8 +820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2061AD1A-F9E1-475E-99DF-2969214ACCAE}">
   <dimension ref="A1:J74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H58" sqref="H58"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I72" sqref="I72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1771,7 +1772,7 @@
       </c>
       <c r="H57" s="49">
         <f>SUM(H58:H62)</f>
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.45">
@@ -1852,7 +1853,9 @@
       <c r="G62" s="40">
         <v>4</v>
       </c>
-      <c r="H62" s="40"/>
+      <c r="H62" s="40">
+        <v>6</v>
+      </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A63" s="28"/>
@@ -1989,14 +1992,14 @@
       <c r="H73" s="32"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A74" s="30"/>
-      <c r="B74" s="30"/>
-      <c r="C74" s="30"/>
-      <c r="D74" s="30"/>
-      <c r="E74" s="30"/>
-      <c r="F74" s="30"/>
-      <c r="G74" s="30"/>
-      <c r="H74" s="30"/>
+      <c r="A74" s="50"/>
+      <c r="B74" s="50"/>
+      <c r="C74" s="50"/>
+      <c r="D74" s="50"/>
+      <c r="E74" s="50"/>
+      <c r="F74" s="50"/>
+      <c r="G74" s="50"/>
+      <c r="H74" s="50"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Finaler Prototyp und Artefakte hochgeladen
</commit_message>
<xml_diff>
--- a/Artefakte/ProjektplanV0.24.xlsx
+++ b/Artefakte/ProjektplanV0.24.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studium\6. Semester\EIS\EISSS19SchoenbergerTissen\Artefakte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A995012D-0869-42EB-A636-131B4F2E8790}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66FFFB3C-AE09-467E-835E-9CE1F71804C9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7950" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{49FFB486-0252-4090-A15B-F7AC9F70B8C0}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{49FFB486-0252-4090-A15B-F7AC9F70B8C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="72">
   <si>
     <t>EIS Projektplan von Malte Schönberger und Arthur Tissen</t>
   </si>
@@ -241,6 +241,12 @@
   </si>
   <si>
     <t>Prototyp (erneut)</t>
+  </si>
+  <si>
+    <t>Client</t>
+  </si>
+  <si>
+    <t>Server</t>
   </si>
 </sst>
 </file>
@@ -818,10 +824,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2061AD1A-F9E1-475E-99DF-2969214ACCAE}">
-  <dimension ref="A1:J74"/>
+  <dimension ref="A1:J76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I72" sqref="I72"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G64" sqref="G64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1879,7 +1885,7 @@
         <v>59</v>
       </c>
       <c r="E64" s="27"/>
-      <c r="F64" s="27"/>
+      <c r="F64" s="34"/>
       <c r="G64" s="27"/>
       <c r="H64" s="27"/>
     </row>
@@ -1887,32 +1893,40 @@
       <c r="A65" s="32"/>
       <c r="B65" s="32"/>
       <c r="C65" s="32"/>
-      <c r="D65" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="E65" s="32"/>
-      <c r="F65" s="32"/>
-      <c r="G65" s="32"/>
-      <c r="H65" s="32"/>
+      <c r="D65" s="32"/>
+      <c r="E65" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="F65" s="45"/>
+      <c r="G65" s="32">
+        <v>120</v>
+      </c>
+      <c r="H65" s="32">
+        <v>180</v>
+      </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A66" s="27"/>
       <c r="B66" s="27"/>
       <c r="C66" s="27"/>
-      <c r="D66" s="27" t="s">
-        <v>60</v>
-      </c>
-      <c r="E66" s="27"/>
-      <c r="F66" s="27"/>
-      <c r="G66" s="27"/>
-      <c r="H66" s="27"/>
+      <c r="D66" s="27"/>
+      <c r="E66" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="F66" s="41"/>
+      <c r="G66" s="27">
+        <v>100</v>
+      </c>
+      <c r="H66" s="27">
+        <v>120</v>
+      </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A67" s="32"/>
       <c r="B67" s="32"/>
       <c r="C67" s="32"/>
       <c r="D67" s="32" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E67" s="32"/>
       <c r="F67" s="32"/>
@@ -1924,82 +1938,134 @@
       <c r="B68" s="27"/>
       <c r="C68" s="27"/>
       <c r="D68" s="27" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E68" s="27"/>
-      <c r="F68" s="27"/>
-      <c r="G68" s="27"/>
-      <c r="H68" s="27"/>
+      <c r="F68" s="38"/>
+      <c r="G68" s="27">
+        <v>8</v>
+      </c>
+      <c r="H68" s="27">
+        <v>6</v>
+      </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A69" s="28"/>
-      <c r="B69" s="28"/>
-      <c r="C69" s="28" t="s">
-        <v>63</v>
-      </c>
-      <c r="D69" s="28"/>
-      <c r="E69" s="28"/>
-      <c r="F69" s="28"/>
-      <c r="G69" s="28"/>
-      <c r="H69" s="28"/>
+      <c r="A69" s="32"/>
+      <c r="B69" s="32"/>
+      <c r="C69" s="32"/>
+      <c r="D69" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="E69" s="32"/>
+      <c r="F69" s="34"/>
+      <c r="G69" s="32">
+        <v>12</v>
+      </c>
+      <c r="H69" s="32">
+        <v>10</v>
+      </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A70" s="27"/>
       <c r="B70" s="27"/>
       <c r="C70" s="27"/>
       <c r="D70" s="27" t="s">
-        <v>27</v>
+        <v>62</v>
       </c>
       <c r="E70" s="27"/>
-      <c r="F70" s="27"/>
-      <c r="G70" s="27"/>
-      <c r="H70" s="27"/>
+      <c r="F70" s="38"/>
+      <c r="G70" s="27">
+        <v>6</v>
+      </c>
+      <c r="H70" s="27">
+        <v>6</v>
+      </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A71" s="32"/>
-      <c r="B71" s="32"/>
-      <c r="C71" s="32"/>
-      <c r="D71" s="32"/>
-      <c r="E71" s="32" t="s">
-        <v>29</v>
-      </c>
-      <c r="F71" s="32"/>
-      <c r="G71" s="32"/>
-      <c r="H71" s="32"/>
+      <c r="A71" s="28"/>
+      <c r="B71" s="28"/>
+      <c r="C71" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="D71" s="28"/>
+      <c r="E71" s="28"/>
+      <c r="F71" s="28"/>
+      <c r="G71" s="28"/>
+      <c r="H71" s="28"/>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A72" s="27"/>
       <c r="B72" s="27"/>
       <c r="C72" s="27"/>
-      <c r="D72" s="27"/>
-      <c r="E72" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="F72" s="27"/>
-      <c r="G72" s="27"/>
-      <c r="H72" s="27"/>
+      <c r="D72" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="E72" s="27"/>
+      <c r="F72" s="34"/>
+      <c r="G72" s="40">
+        <v>12</v>
+      </c>
+      <c r="H72" s="40">
+        <v>12</v>
+      </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A73" s="32"/>
       <c r="B73" s="32"/>
       <c r="C73" s="32"/>
-      <c r="D73" s="32" t="s">
+      <c r="D73" s="32"/>
+      <c r="E73" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="F73" s="34"/>
+      <c r="G73" s="39">
+        <v>4</v>
+      </c>
+      <c r="H73" s="39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A74" s="27"/>
+      <c r="B74" s="27"/>
+      <c r="C74" s="27"/>
+      <c r="D74" s="27"/>
+      <c r="E74" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="F74" s="34"/>
+      <c r="G74" s="40">
+        <v>6</v>
+      </c>
+      <c r="H74" s="40">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A75" s="32"/>
+      <c r="B75" s="32"/>
+      <c r="C75" s="32"/>
+      <c r="D75" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="E73" s="32"/>
-      <c r="F73" s="32"/>
-      <c r="G73" s="32"/>
-      <c r="H73" s="32"/>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A74" s="50"/>
-      <c r="B74" s="50"/>
-      <c r="C74" s="50"/>
-      <c r="D74" s="50"/>
-      <c r="E74" s="50"/>
-      <c r="F74" s="50"/>
-      <c r="G74" s="50"/>
-      <c r="H74" s="50"/>
+      <c r="E75" s="32"/>
+      <c r="F75" s="34"/>
+      <c r="G75" s="48">
+        <v>1</v>
+      </c>
+      <c r="H75" s="48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A76" s="50"/>
+      <c r="B76" s="50"/>
+      <c r="C76" s="50"/>
+      <c r="D76" s="50"/>
+      <c r="E76" s="50"/>
+      <c r="F76" s="50"/>
+      <c r="G76" s="50"/>
+      <c r="H76" s="50"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>